<commit_message>
fix: revert admin dev default; seed customers only when table empty; autosave on customer select when hours/day present
</commit_message>
<xml_diff>
--- a/labor-timekeeper/exports/2025-12/2025-12-29/Boban_Abbate_2025-12-29.xlsx
+++ b/labor-timekeeper/exports/2025-12/2025-12-29/Boban_Abbate_2025-12-29.xlsx
@@ -5,13 +5,14 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="Weekly Timesheet" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Jason Schema" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -31,10 +32,19 @@
     <t>Total</t>
   </si>
   <si>
+    <t>2026-01-01</t>
+  </si>
+  <si>
+    <t>Evans</t>
+  </si>
+  <si>
+    <t>Holiday</t>
+  </si>
+  <si>
     <t>2026-01-02</t>
   </si>
   <si>
-    <t>Tattersall</t>
+    <t>Oglesby</t>
   </si>
   <si>
     <t>Regular</t>
@@ -46,10 +56,34 @@
     <t/>
   </si>
   <si>
-    <t>Reg: 7 / OT: 0</t>
+    <t>Reg: 40 / OT: 0</t>
   </si>
   <si>
     <t>Category: HOURLY</t>
+  </si>
+  <si>
+    <t>HOURLY SUBTOTAL</t>
+  </si>
+  <si>
+    <t>ADMIN SUBTOTAL</t>
+  </si>
+  <si>
+    <t>GRAND TOTAL</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Employee ID</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Boban Abbate</t>
+  </si>
+  <si>
+    <t>emp_pw6be4hd</t>
   </si>
 </sst>
 </file>
@@ -59,7 +93,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -70,8 +104,12 @@
     <font>
       <b/>
     </font>
+    <font>
+      <b/>
+      <color rgb="FF0000"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,6 +126,16 @@
         <fgColor rgb="FFFFE0B0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAF3E0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8F8E0"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -101,13 +149,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,7 +501,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F10"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
@@ -486,56 +540,245 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="1">
-        <v>42.5</v>
+        <v>0</v>
       </c>
       <c r="F2" s="1">
-        <v>297.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4">
+        <v>40</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="5">
-        <v>297.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>10</v>
+      <c r="I3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: simulator full-month coverage, persist logs, fix employees
</commit_message>
<xml_diff>
--- a/labor-timekeeper/exports/2025-12/2025-12-29/Boban_Abbate_2025-12-29.xlsx
+++ b/labor-timekeeper/exports/2025-12/2025-12-29/Boban_Abbate_2025-12-29.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -35,16 +35,13 @@
     <t>2026-01-01</t>
   </si>
   <si>
-    <t>Evans</t>
-  </si>
-  <si>
-    <t>Holiday</t>
+    <t>PTO</t>
   </si>
   <si>
     <t>2026-01-02</t>
   </si>
   <si>
-    <t>Oglesby</t>
+    <t>Muncey</t>
   </si>
   <si>
     <t>Regular</t>
@@ -56,7 +53,7 @@
     <t/>
   </si>
   <si>
-    <t>Reg: 40 / OT: 0</t>
+    <t>Reg: 24 / OT: 0</t>
   </si>
   <si>
     <t>Category: HOURLY</t>
@@ -83,7 +80,7 @@
     <t>Boban Abbate</t>
   </si>
   <si>
-    <t>emp_pw6be4hd</t>
+    <t>emp_ga4rqytu</t>
   </si>
 </sst>
 </file>
@@ -540,113 +537,113 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="F2" s="1">
-        <v>0</v>
+        <v>1760</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="C3">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="F3" s="1">
-        <v>0</v>
+        <v>880</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4">
+        <v>24</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="4">
-        <v>40</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="E5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="5">
-        <v>0</v>
+        <v>2640</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" s="7">
-        <v>0</v>
+        <v>2640</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9" s="7">
         <v>0</v>
@@ -654,22 +651,22 @@
     </row>
     <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10" s="9">
-        <v>0</v>
+        <v>2640</v>
       </c>
     </row>
   </sheetData>
@@ -696,10 +693,10 @@
   <sheetData>
     <row r="1" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>20</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>0</v>
@@ -720,15 +717,15 @@
         <v>3</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
         <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -737,48 +734,48 @@
         <v>7</v>
       </c>
       <c r="E2">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F2" s="1">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="G2" s="1">
-        <v>0</v>
+        <v>1760</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1">
+        <v>110</v>
+      </c>
+      <c r="G3" s="1">
+        <v>880</v>
+      </c>
+      <c r="H3" t="s">
         <v>10</v>
       </c>
-      <c r="E3">
-        <v>20</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: save local exports and scripts
</commit_message>
<xml_diff>
--- a/labor-timekeeper/exports/2025-12/2025-12-29/Boban_Abbate_2025-12-29.xlsx
+++ b/labor-timekeeper/exports/2025-12/2025-12-29/Boban_Abbate_2025-12-29.xlsx
@@ -5,51 +5,79 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="Weekly Timesheet" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Jason Schema" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
   <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>2026-01-02</t>
+  </si>
+  <si>
+    <t>Montross</t>
+  </si>
+  <si>
+    <t>Regular</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>SUBTOTAL</t>
+  </si>
+  <si>
+    <t>Reg: 10 / OT: 0</t>
+  </si>
+  <si>
+    <t>Category: HOURLY</t>
+  </si>
+  <si>
+    <t>HOURLY SUBTOTAL</t>
+  </si>
+  <si>
+    <t>ADMIN SUBTOTAL</t>
+  </si>
+  <si>
+    <t>GRAND TOTAL</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Employee ID</t>
+  </si>
+  <si>
     <t>Client</t>
   </si>
   <si>
-    <t>Hours</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Rate</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>2026-01-02</t>
-  </si>
-  <si>
-    <t>Tattersall</t>
-  </si>
-  <si>
-    <t>Regular</t>
-  </si>
-  <si>
-    <t>SUBTOTAL</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Reg: 7 / OT: 0</t>
-  </si>
-  <si>
-    <t>Category: HOURLY</t>
+    <t>Boban Abbate</t>
+  </si>
+  <si>
+    <t>emp_ga4rqytu</t>
   </si>
 </sst>
 </file>
@@ -59,7 +87,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -70,8 +98,12 @@
     <font>
       <b/>
     </font>
+    <font>
+      <b/>
+      <color rgb="FF0000"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -80,16 +112,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE0E0E0"/>
+        <fgColor rgb="FFD9E1F2"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFE0B0"/>
+        <fgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAF3E0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8F8E0"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -97,17 +139,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,94 +535,262 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="8" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="6" width="12" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="6">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="7">
+        <v>110</v>
+      </c>
+      <c r="F2" s="7">
+        <v>1100</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="10">
+        <v>10</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="12">
+        <v>1100</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="17">
+        <v>1100</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="17">
+        <v>0</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="21">
+        <v>1100</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="2" width="14" customWidth="1"/>
+    <col min="3" max="5" width="12" customWidth="1"/>
+    <col min="6" max="7" width="12" style="1" customWidth="1"/>
+    <col min="8" max="9" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1">
-        <v>42.5</v>
-      </c>
-      <c r="F2" s="1">
-        <v>297.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="E2" s="6">
+        <v>10</v>
+      </c>
+      <c r="F2" s="7">
+        <v>110</v>
+      </c>
+      <c r="G2" s="7">
+        <v>1100</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4">
-        <v>7</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="5">
-        <v>297.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="I2" s="5" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>